<commit_message>
Implementa melhorias no menu de Utilitários: adiciona barra de pesquisa, filtro de status funcional e remove botão toggle confuso
</commit_message>
<xml_diff>
--- a/Descrição de Planos.xlsx
+++ b/Descrição de Planos.xlsx
@@ -8,26 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjetoForgeLock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B544D92F-A204-4BEE-B232-D3A61E33D4FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5074D203-406C-4275-8451-317725D8C92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28380" yWindow="2415" windowWidth="20655" windowHeight="17910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="1515" windowWidth="20655" windowHeight="17910" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gostei dos nomes Básico, Pro e " sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Funcionalidade</t>
   </si>
   <si>
-    <t>Plano Básico</t>
-  </si>
-  <si>
     <t>Plano Pro</t>
   </si>
   <si>
@@ -74,13 +85,28 @@
   </si>
   <si>
     <t>Ilimitado (Clientes, Produtos, Projetos)</t>
+  </si>
+  <si>
+    <t>Plano Basic</t>
+  </si>
+  <si>
+    <t>tabelas:</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>cadastro do tipo do plano e campos de controle</t>
+  </si>
+  <si>
+    <t>planprice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -90,6 +116,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -115,7 +148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -128,6 +161,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -347,10 +383,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -365,32 +401,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -404,44 +440,101 @@
     </row>
     <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="122.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFB4C773-7733-4382-8149-CEFF1BFE85A9}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>40</v>
+      </c>
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1">
+        <f>A1/B1</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>